<commit_message>
adesão de verificação de pesquisa específica, mudança de paths e prints no terminal
</commit_message>
<xml_diff>
--- a/planilhas/Resultado (modelo).xlsx
+++ b/planilhas/Resultado (modelo).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuário\Desktop\code\python\bots\planilhas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuário\Desktop\code\python\bots\bot-web-cras\planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD6FDFE-E911-4BD6-91BA-77188C086D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FC62F4-D387-4A80-9BFD-0F4008F31B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>ID CRAS</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>COMENTÁRIO</t>
+  </si>
+  <si>
+    <t>DATA E HORÁRIO DA EXTRAÇÃO</t>
   </si>
 </sst>
 </file>
@@ -396,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,9 +414,10 @@
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,6 +438,9 @@
       </c>
       <c r="G1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
criação de um bot "reduzido" e adição no caso de correspondência parcial e contagem do idcras
</commit_message>
<xml_diff>
--- a/planilhas/Resultado (modelo).xlsx
+++ b/planilhas/Resultado (modelo).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuário\Desktop\code\python\bots\bot-web-cras\planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FC62F4-D387-4A80-9BFD-0F4008F31B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BB2870-474B-49BD-B85B-1FF896C78D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>ID CRAS</t>
   </si>
@@ -29,6 +29,12 @@
     <t>NOME</t>
   </si>
   <si>
+    <t>CIDADE</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
     <t>ENDEREÇO</t>
   </si>
   <si>
@@ -44,6 +50,9 @@
     <t>NOTA</t>
   </si>
   <si>
+    <t>DATA E HORÁRIO DA EXTRAÇÃO</t>
+  </si>
+  <si>
     <t>ID COMENTÁRIO</t>
   </si>
   <si>
@@ -57,9 +66,6 @@
   </si>
   <si>
     <t>COMENTÁRIO</t>
-  </si>
-  <si>
-    <t>DATA E HORÁRIO DA EXTRAÇÃO</t>
   </si>
 </sst>
 </file>
@@ -399,25 +405,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A2" sqref="A2:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,7 +448,13 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -453,18 +467,18 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -475,19 +489,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mudança de nomes de variáveis e correção no modo de armazenar o link do maps
</commit_message>
<xml_diff>
--- a/planilhas/Resultado (modelo).xlsx
+++ b/planilhas/Resultado (modelo).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuário\Desktop\code\python\bots\bot-web-cras\planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BB2870-474B-49BD-B85B-1FF896C78D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB160A9F-16F6-4308-9D7D-923289F36EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -407,21 +407,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="70.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -467,18 +467,18 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>